<commit_message>
adjusted backgrond color on the boxplot. added a chart for differences between average calculated and actual distance.
</commit_message>
<xml_diff>
--- a/ble-single-antenna-distance-detection-accuracy/Statistics Charts.xlsx
+++ b/ble-single-antenna-distance-detection-accuracy/Statistics Charts.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
   <si>
     <t>Horizontal Label</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Average Distance</t>
+  </si>
+  <si>
+    <t>ABS Difference</t>
   </si>
 </sst>
 </file>
@@ -94,7 +97,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -108,6 +111,9 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
     </font>
   </fonts>
   <fills count="2">
@@ -124,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -135,12 +141,27 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="2" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -273,11 +294,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="395617980"/>
-        <c:axId val="996178837"/>
+        <c:axId val="1847027562"/>
+        <c:axId val="1864659092"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="395617980"/>
+        <c:axId val="1847027562"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -329,10 +350,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="996178837"/>
+        <c:crossAx val="1864659092"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="996178837"/>
+        <c:axId val="1864659092"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -407,7 +428,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="395617980"/>
+        <c:crossAx val="1847027562"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -525,11 +546,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1581537771"/>
-        <c:axId val="2141552983"/>
+        <c:axId val="523564053"/>
+        <c:axId val="519595776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1581537771"/>
+        <c:axId val="523564053"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -581,10 +602,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2141552983"/>
+        <c:crossAx val="519595776"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2141552983"/>
+        <c:axId val="519595776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -659,7 +680,341 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1581537771"/>
+        <c:crossAx val="523564053"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" sz="1800">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1800">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Absolute Difference between Average Calculated and Actual Distance</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="4285F4"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="15"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="16"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="17"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="18"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+          </c:dPt>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Average vs Actual'!$A$2:$A$20</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Average vs Actual'!$D$2:$D$20</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="752234261"/>
+        <c:axId val="100486646"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="752234261"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Actual Distance</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="100486646"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="100486646"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Difference in Meters</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="752234261"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -719,8 +1074,8 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
@@ -737,6 +1092,31 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3533775"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 3" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1265,217 +1645,301 @@
       <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="D1" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="7">
         <v>0.5</v>
       </c>
       <c r="C2" s="5">
         <v>1.05858</v>
+      </c>
+      <c r="D2" s="8">
+        <f t="shared" ref="D2:D20" si="1">ABS(B2 - C2)</f>
+        <v>0.55858</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="7">
         <v>1.0</v>
       </c>
       <c r="C3" s="5">
         <v>1.334375</v>
+      </c>
+      <c r="D3" s="8">
+        <f t="shared" si="1"/>
+        <v>0.334375</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="7">
         <v>1.5</v>
       </c>
       <c r="C4" s="5">
         <v>1.512985</v>
+      </c>
+      <c r="D4" s="8">
+        <f t="shared" si="1"/>
+        <v>0.012985</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="7">
         <v>2.0</v>
       </c>
       <c r="C5" s="5">
         <v>2.100825</v>
+      </c>
+      <c r="D5" s="8">
+        <f t="shared" si="1"/>
+        <v>0.100825</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="7">
         <v>2.5</v>
       </c>
       <c r="C6" s="5">
         <v>1.69501</v>
+      </c>
+      <c r="D6" s="8">
+        <f t="shared" si="1"/>
+        <v>0.80499</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="7">
         <v>3.0</v>
       </c>
       <c r="C7" s="5">
         <v>1.610535</v>
+      </c>
+      <c r="D7" s="8">
+        <f t="shared" si="1"/>
+        <v>1.389465</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="7">
         <v>3.5</v>
       </c>
       <c r="C8" s="5">
         <v>2.749795</v>
+      </c>
+      <c r="D8" s="8">
+        <f t="shared" si="1"/>
+        <v>0.750205</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="7">
         <v>4.0</v>
       </c>
       <c r="C9" s="5">
         <v>2.756665</v>
+      </c>
+      <c r="D9" s="8">
+        <f t="shared" si="1"/>
+        <v>1.243335</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="7">
         <v>4.5</v>
       </c>
       <c r="C10" s="5">
         <v>2.726235</v>
+      </c>
+      <c r="D10" s="8">
+        <f t="shared" si="1"/>
+        <v>1.773765</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="7">
         <v>5.0</v>
       </c>
       <c r="C11" s="5">
         <v>2.17584</v>
+      </c>
+      <c r="D11" s="8">
+        <f t="shared" si="1"/>
+        <v>2.82416</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="7">
         <v>5.5</v>
       </c>
       <c r="C12" s="5">
         <v>3.310665</v>
+      </c>
+      <c r="D12" s="8">
+        <f t="shared" si="1"/>
+        <v>2.189335</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="7">
         <v>6.0</v>
       </c>
       <c r="C13" s="5">
         <v>3.89448</v>
+      </c>
+      <c r="D13" s="8">
+        <f t="shared" si="1"/>
+        <v>2.10552</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="7">
         <v>6.5</v>
       </c>
       <c r="C14" s="5">
         <v>3.60135</v>
+      </c>
+      <c r="D14" s="8">
+        <f t="shared" si="1"/>
+        <v>2.89865</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="7">
         <v>7.0</v>
       </c>
       <c r="C15" s="5">
         <v>2.590705</v>
+      </c>
+      <c r="D15" s="8">
+        <f t="shared" si="1"/>
+        <v>4.409295</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="7">
         <v>7.5</v>
       </c>
       <c r="C16" s="5">
         <v>4.912985</v>
+      </c>
+      <c r="D16" s="8">
+        <f t="shared" si="1"/>
+        <v>2.587015</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="7">
         <v>8.0</v>
       </c>
       <c r="C17" s="5">
         <v>2.42328</v>
+      </c>
+      <c r="D17" s="8">
+        <f t="shared" si="1"/>
+        <v>5.57672</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="7">
         <v>8.5</v>
       </c>
       <c r="C18" s="5">
         <v>3.67317</v>
+      </c>
+      <c r="D18" s="8">
+        <f t="shared" si="1"/>
+        <v>4.82683</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="7">
         <v>9.0</v>
       </c>
       <c r="C19" s="5">
         <v>2.967425</v>
+      </c>
+      <c r="D19" s="8">
+        <f t="shared" si="1"/>
+        <v>6.032575</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="7">
         <v>9.5</v>
       </c>
       <c r="C20" s="5">
         <v>4.494755</v>
       </c>
+      <c r="D20" s="8">
+        <f t="shared" si="1"/>
+        <v>5.005245</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D2:D20">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
reformatted the calculated statistics table
</commit_message>
<xml_diff>
--- a/ble-single-antenna-distance-detection-accuracy/Statistics Charts.xlsx
+++ b/ble-single-antenna-distance-detection-accuracy/Statistics Charts.xlsx
@@ -294,11 +294,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1847027562"/>
-        <c:axId val="1864659092"/>
+        <c:axId val="356387682"/>
+        <c:axId val="259153022"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1847027562"/>
+        <c:axId val="356387682"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -350,10 +350,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1864659092"/>
+        <c:crossAx val="259153022"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1864659092"/>
+        <c:axId val="259153022"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -428,7 +428,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1847027562"/>
+        <c:crossAx val="356387682"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -546,11 +546,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="523564053"/>
-        <c:axId val="519595776"/>
+        <c:axId val="936517890"/>
+        <c:axId val="1362676805"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="523564053"/>
+        <c:axId val="936517890"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -602,10 +602,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="519595776"/>
+        <c:crossAx val="1362676805"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="519595776"/>
+        <c:axId val="1362676805"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -680,7 +680,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="523564053"/>
+        <c:crossAx val="936517890"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -880,11 +880,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="752234261"/>
-        <c:axId val="100486646"/>
+        <c:axId val="2052138929"/>
+        <c:axId val="1648498605"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="752234261"/>
+        <c:axId val="2052138929"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -936,10 +936,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100486646"/>
+        <c:crossAx val="1648498605"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100486646"/>
+        <c:axId val="1648498605"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1014,7 +1014,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="752234261"/>
+        <c:crossAx val="2052138929"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>

</xml_diff>